<commit_message>
QAPF map area 1_J
</commit_message>
<xml_diff>
--- a/_CIPW/CIPW/AREA1_J/QAPF_counts.xlsx
+++ b/_CIPW/CIPW/AREA1_J/QAPF_counts.xlsx
@@ -380,7 +380,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>41325</v>
+        <v>42365</v>
       </c>
     </row>
     <row r="3">
@@ -390,7 +390,7 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>1309</v>
+        <v>473</v>
       </c>
     </row>
     <row r="4">
@@ -401,7 +401,7 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>676</v>
+        <v>472</v>
       </c>
     </row>
   </sheetData>

</xml_diff>